<commit_message>
fixed all unittests and smaller bugs
</commit_message>
<xml_diff>
--- a/sbmlutils/examples/models/demo/demo_annotations.xlsx
+++ b/sbmlutils/examples/models/demo/demo_annotations.xlsx
@@ -5,220 +5,225 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="183" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="68">
   <si>
-    <t>pattern</t>
-  </si>
-  <si>
-    <t>sbml_type</t>
-  </si>
-  <si>
-    <t>annotation_type</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>qualifier</t>
-  </si>
-  <si>
-    <t>collection</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>#model</t>
-  </si>
-  <si>
-    <t>document</t>
-  </si>
-  <si>
-    <t>RDF</t>
-  </si>
-  <si>
-    <t>SBO:0000293</t>
-  </si>
-  <si>
-    <t>BQM_IS</t>
-  </si>
-  <si>
-    <t>biomodels.sbo</t>
-  </si>
-  <si>
-    <t>non-spatial continuous framework</t>
-  </si>
-  <si>
-    <t>^demo_\d+$</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>GO:0008152</t>
-  </si>
-  <si>
-    <t>go</t>
-  </si>
-  <si>
-    <t>metabolic process</t>
-  </si>
-  <si>
-    <t># compartment</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>compartment</t>
-  </si>
-  <si>
-    <t>SBO:0000290</t>
-  </si>
-  <si>
-    <t>BQB_IS</t>
-  </si>
-  <si>
-    <t>physical compartment</t>
-  </si>
-  <si>
-    <t>GO:0005615</t>
-  </si>
-  <si>
-    <t>extracellular space</t>
-  </si>
-  <si>
-    <t>FMA:70022</t>
-  </si>
-  <si>
-    <t>fma</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>GO:0005886</t>
-  </si>
-  <si>
-    <t>plasma membrane</t>
-  </si>
-  <si>
-    <t>FMA:63841</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>GO:0005623</t>
-  </si>
-  <si>
-    <t>cell</t>
-  </si>
-  <si>
-    <t>FMA:68646</t>
-  </si>
-  <si>
-    <t># parameters</t>
-  </si>
-  <si>
-    <t>^Km_\w+$</t>
-  </si>
-  <si>
-    <t>parameter</t>
-  </si>
-  <si>
-    <t>SBO:0000027</t>
-  </si>
-  <si>
-    <t>Michaelis constant</t>
-  </si>
-  <si>
-    <t>^Keq_\w+$</t>
-  </si>
-  <si>
-    <t>SBO:0000281</t>
-  </si>
-  <si>
-    <t>equilibrium constant</t>
-  </si>
-  <si>
-    <t>^Vmax_\w+$</t>
-  </si>
-  <si>
-    <t>SBO:0000186</t>
-  </si>
-  <si>
-    <t>maximal velocity</t>
-  </si>
-  <si>
-    <t># species</t>
-  </si>
-  <si>
-    <t>^\w{1}__A$</t>
-  </si>
-  <si>
-    <t>species</t>
-  </si>
-  <si>
-    <t>SBO:0000247</t>
-  </si>
-  <si>
-    <t>simple chemical</t>
-  </si>
-  <si>
-    <t>^\w{1}__B$</t>
-  </si>
-  <si>
-    <t>^\w{1}__C$</t>
-  </si>
-  <si>
-    <t>^\w{1}__\w+$</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>C6H12O6</t>
-  </si>
-  <si>
-    <t>Charge</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t># reactions</t>
-  </si>
-  <si>
-    <t>^b\w{1}$</t>
-  </si>
-  <si>
-    <t>reaction</t>
-  </si>
-  <si>
-    <t>SBO:0000185</t>
-  </si>
-  <si>
-    <t>transport reaction</t>
-  </si>
-  <si>
-    <t>^v\w{1}$</t>
-  </si>
-  <si>
-    <t>SBO:0000176</t>
-  </si>
-  <si>
-    <t>biochemical reaction</t>
+    <t xml:space="preserve">pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sbml_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annotation_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qualifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQM_IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sbo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">non-spatial continuous framework</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^demo_\d+$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0008152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metabolic process</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BQB_IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">physical compartment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005615</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extracellular space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMA:70022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plasma membrane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMA:63841</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005623</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMA:68646</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^Km_\w+$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parameter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000027</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michaelis constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^Keq_\w+$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equilibrium constant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^Vmax_\w+$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maximal velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^\w{1}__A$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">species</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simple chemical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^\w{1}__B$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^\w{1}__C$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^\w{1}__\w+$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6H12O6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># reactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^b\w{1}$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transport reaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^v\w{1}$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBO:0000176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">biochemical reaction</t>
   </si>
 </sst>
 </file>
@@ -226,10 +231,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -265,13 +270,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -334,7 +332,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,10 +394,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,14 +477,19 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="18.7448979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.46938775510204"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.7448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.9132653061224"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="18.7448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="18.7448979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -503,13 +502,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -522,12 +521,12 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7"/>
       <c r="B3" s="8" t="s">
         <v>8</v>
@@ -535,20 +534,20 @@
       <c r="C3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
@@ -558,13 +557,13 @@
       <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -586,12 +585,12 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
@@ -601,20 +600,20 @@
       <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
@@ -624,20 +623,20 @@
       <c r="C8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
@@ -647,13 +646,13 @@
       <c r="C9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -669,7 +668,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>29</v>
       </c>
@@ -679,20 +678,20 @@
       <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>29</v>
       </c>
@@ -702,20 +701,20 @@
       <c r="C12" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>30</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>29</v>
       </c>
@@ -725,14 +724,14 @@
       <c r="C13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>31</v>
@@ -747,7 +746,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>33</v>
       </c>
@@ -757,20 +756,20 @@
       <c r="C15" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
@@ -780,20 +779,20 @@
       <c r="C16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -803,14 +802,14 @@
       <c r="C17" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>35</v>
@@ -820,9 +819,9 @@
       <c r="A18" s="0"/>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="0"/>
-      <c r="F18" s="9"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
       <c r="G18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,12 +830,12 @@
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
@@ -846,20 +845,20 @@
       <c r="C20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
         <v>42</v>
       </c>
@@ -869,20 +868,20 @@
       <c r="C21" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>43</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
@@ -892,14 +891,14 @@
       <c r="C22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>47</v>
@@ -920,12 +919,12 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -935,20 +934,20 @@
       <c r="C25" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
         <v>53</v>
       </c>
@@ -958,20 +957,20 @@
       <c r="C26" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="s">
         <v>54</v>
       </c>
@@ -981,21 +980,21 @@
       <c r="C27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B28" s="9" t="s">
@@ -1004,15 +1003,15 @@
       <c r="C28" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="0"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="0"/>
-      <c r="F28" s="9"/>
       <c r="G28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -1021,11 +1020,11 @@
       <c r="C29" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
       <c r="G29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1034,12 +1033,12 @@
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
@@ -1049,20 +1048,20 @@
       <c r="C31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="D31" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="E31" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G31" s="15" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="7" t="s">
         <v>65</v>
       </c>
@@ -1072,14 +1071,14 @@
       <c r="C32" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G32" s="15" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
working on annotation fix
</commit_message>
<xml_diff>
--- a/sbmlutils/examples/models/demo/demo_annotations.xlsx
+++ b/sbmlutils/examples/models/demo/demo_annotations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Annotation" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -37,19 +37,19 @@
     <t xml:space="preserve">collection</t>
   </si>
   <si>
-    <t xml:space="preserve">entity</t>
+    <t xml:space="preserve">resource</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">#model</t>
+    <t xml:space="preserve"># model</t>
   </si>
   <si>
     <t xml:space="preserve">document</t>
   </si>
   <si>
-    <t xml:space="preserve">RDF</t>
+    <t xml:space="preserve">rdf</t>
   </si>
   <si>
     <t xml:space="preserve">BQM_IS</t>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">sbo</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000293</t>
+    <t xml:space="preserve">sbo/SBO:0000293</t>
   </si>
   <si>
     <t xml:space="preserve">non-spatial continuous framework</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">go</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0008152</t>
+    <t xml:space="preserve">go/GO:0008152</t>
   </si>
   <si>
     <t xml:space="preserve">metabolic process</t>
@@ -91,13 +91,13 @@
     <t xml:space="preserve">BQB_IS</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000290</t>
+    <t xml:space="preserve">sbo/SBO:0000290</t>
   </si>
   <si>
     <t xml:space="preserve">physical compartment</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005615</t>
+    <t xml:space="preserve">go/GO:0005615</t>
   </si>
   <si>
     <t xml:space="preserve">extracellular space</t>
@@ -106,31 +106,31 @@
     <t xml:space="preserve">fma</t>
   </si>
   <si>
-    <t xml:space="preserve">FMA:70022</t>
+    <t xml:space="preserve">fma/FMA:70022</t>
   </si>
   <si>
     <t xml:space="preserve">m</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005886</t>
+    <t xml:space="preserve">go/GO:0005886</t>
   </si>
   <si>
     <t xml:space="preserve">plasma membrane</t>
   </si>
   <si>
-    <t xml:space="preserve">FMA:63841</t>
+    <t xml:space="preserve">fma/FMA:63841</t>
   </si>
   <si>
     <t xml:space="preserve">c</t>
   </si>
   <si>
-    <t xml:space="preserve">GO:0005623</t>
+    <t xml:space="preserve">go/GO:0005623</t>
   </si>
   <si>
     <t xml:space="preserve">cell</t>
   </si>
   <si>
-    <t xml:space="preserve">FMA:68646</t>
+    <t xml:space="preserve">fma/FMA:68646</t>
   </si>
   <si>
     <t xml:space="preserve"># parameters</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">parameter</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000027</t>
+    <t xml:space="preserve">sbo/SBO:0000027</t>
   </si>
   <si>
     <t xml:space="preserve">Michaelis constant</t>
@@ -151,7 +151,7 @@
     <t xml:space="preserve">^Keq_\w+$</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000281</t>
+    <t xml:space="preserve">sbo/SBO:0000281</t>
   </si>
   <si>
     <t xml:space="preserve">equilibrium constant</t>
@@ -160,7 +160,7 @@
     <t xml:space="preserve">^Vmax_\w+$</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000186</t>
+    <t xml:space="preserve">sbo/SBO:0000186</t>
   </si>
   <si>
     <t xml:space="preserve">maximal velocity</t>
@@ -175,7 +175,7 @@
     <t xml:space="preserve">species</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000247</t>
+    <t xml:space="preserve">sbo/SBO:0000247</t>
   </si>
   <si>
     <t xml:space="preserve">simple chemical</t>
@@ -190,13 +190,13 @@
     <t xml:space="preserve">^\w{1}__\w+$</t>
   </si>
   <si>
-    <t xml:space="preserve">Formula</t>
+    <t xml:space="preserve">formula</t>
   </si>
   <si>
     <t xml:space="preserve">C6H12O6</t>
   </si>
   <si>
-    <t xml:space="preserve">Charge</t>
+    <t xml:space="preserve">charge</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000185</t>
+    <t xml:space="preserve">sbo/SBO:0000185</t>
   </si>
   <si>
     <t xml:space="preserve">transport reaction</t>
@@ -220,7 +220,7 @@
     <t xml:space="preserve">^v\w{1}$</t>
   </si>
   <si>
-    <t xml:space="preserve">SBO:0000176</t>
+    <t xml:space="preserve">sbo/SBO:0000176</t>
   </si>
   <si>
     <t xml:space="preserve">biochemical reaction</t>
@@ -477,19 +477,19 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F52" activeCellId="0" sqref="F52"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="18.7448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.46938775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.7448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="31.9132653061224"/>
-    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="18.7448979591837"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="18.7448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="19.1428571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.1428571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="32.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1023" min="8" style="1" width="19.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="19.1428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>